<commit_message>
Updated CoG Er Raman
Thanks Yonis
</commit_message>
<xml_diff>
--- a/CoG Data.xlsx
+++ b/CoG Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19735\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\y.ochoaozoria\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E607AC9-8B41-42D3-9578-EA318474CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2905FA14-B5AA-41E8-B491-23FCDB2977A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3858B844-7A3D-40F6-BFE1-713DCA587643}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{3858B844-7A3D-40F6-BFE1-713DCA587643}"/>
   </bookViews>
   <sheets>
     <sheet name="Pr Fluorescence" sheetId="1" r:id="rId1"/>
     <sheet name="Raman" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,30 +51,6 @@
     <t>Aberration</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Edge (nm)</t>
-  </si>
-  <si>
-    <t>Center (nm)</t>
-  </si>
-  <si>
-    <t>Glass Avg (nm)</t>
-  </si>
-  <si>
-    <t>Crystal Avg (nm)</t>
-  </si>
-  <si>
-    <t>r_x (um)</t>
-  </si>
-  <si>
-    <t>r_y (um)</t>
-  </si>
-  <si>
     <t>Speed (um/s)</t>
   </si>
   <si>
@@ -84,19 +60,40 @@
     <t>Depth (um)</t>
   </si>
   <si>
+    <t>Glass Avg (nm)</t>
+  </si>
+  <si>
+    <t>Crystal Avg (nm)</t>
+  </si>
+  <si>
     <t>Dif (nm)</t>
   </si>
   <si>
-    <t>Sample</t>
+    <t>Edge (nm)</t>
   </si>
   <si>
-    <t>Pr 1</t>
+    <t>Center (nm)</t>
   </si>
   <si>
-    <t>Er 1</t>
+    <t>r_x (um)</t>
   </si>
   <si>
-    <t>Er 4</t>
+    <t>r_y (um)</t>
+  </si>
+  <si>
+    <t>Crystal Area (um^2)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
   <si>
     <t>Glass Avg (1/cm)</t>
@@ -114,23 +111,26 @@
     <t>Center (1/cm)</t>
   </si>
   <si>
-    <t>Crystal Area (um^2)</t>
-  </si>
-  <si>
     <t>Raman</t>
   </si>
   <si>
-    <t>Fluorescence</t>
+    <t>Pr 1</t>
   </si>
   <si>
-    <t>Peak</t>
+    <t>Er 1</t>
+  </si>
+  <si>
+    <t>Er 4</t>
+  </si>
+  <si>
+    <t>Fluorescence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +248,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,10 +264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,12 +580,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574E1FA4-26B4-45A7-A185-512A8100C98F}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -605,7 +605,7 @@
     <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -619,62 +619,62 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="13">
         <v>0.2</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="11">
+      <c r="E2" s="13">
+        <v>15</v>
+      </c>
+      <c r="F2" s="13">
         <v>650</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="13">
         <v>600</v>
       </c>
       <c r="H2" s="3">
@@ -707,16 +707,16 @@
         <v>238.5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:16">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="3">
         <v>607.28646352739804</v>
       </c>
@@ -747,58 +747,58 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:16">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13">
         <v>740</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="15">
+      <c r="G4" s="13"/>
+      <c r="H4" s="11">
         <v>607.34140000000002</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="11">
         <v>4371950.2244032398</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>-4371342.8830032395</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="11">
         <v>607.28149808077796</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="11">
         <v>607.35987198642295</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="11">
         <f t="shared" si="1"/>
         <v>-7.8373905644980368E-2</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="11">
         <v>14.75</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="11">
         <v>29.5</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="12">
         <v>1799.75</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:16">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="2">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="3">
         <v>607.28625616569798</v>
       </c>
@@ -829,16 +829,16 @@
         <v>318.25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:16">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2">
         <v>8</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13">
         <v>300</v>
       </c>
       <c r="H6" s="3">
@@ -871,16 +871,16 @@
         <v>338.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:16">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="2">
         <v>9</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="3">
         <v>607.29026325795098</v>
       </c>
@@ -911,18 +911,18 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+    <row r="8" spans="1:16">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2">
         <v>11</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
         <v>650</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="3">
         <v>607.28709332677499</v>
       </c>
@@ -953,16 +953,16 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+    <row r="9" spans="1:16">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2">
         <v>12</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="3">
         <v>607.28752045176805</v>
       </c>
@@ -993,24 +993,24 @@
         <v>328</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11">
+    <row r="10" spans="1:16">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13">
         <v>2</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>5</v>
+      <c r="D10" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E10" s="2">
         <v>20</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="13">
         <v>325</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="13">
         <v>1200</v>
       </c>
       <c r="H10" s="3">
@@ -1043,18 +1043,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+    <row r="11" spans="1:16">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="2">
         <v>25</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="3">
         <v>607.28422778109802</v>
       </c>
@@ -1085,20 +1085,20 @@
         <v>97.25</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+    <row r="12" spans="1:16">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="2">
         <v>7</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="2">
         <v>20</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="13">
         <v>400</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="3">
         <v>607.11601330353596</v>
       </c>
@@ -1129,18 +1129,18 @@
         <v>246.5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+    <row r="13" spans="1:16">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="2">
         <v>9</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="2">
         <v>25</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="3">
         <v>607.28285326792695</v>
       </c>
@@ -1171,20 +1171,20 @@
         <v>161.25</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+    <row r="14" spans="1:16">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="2">
         <v>11</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2">
         <v>20</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="13">
         <v>400</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="13">
         <v>600</v>
       </c>
       <c r="H14" s="3">
@@ -1217,18 +1217,18 @@
         <v>205.75</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+    <row r="15" spans="1:16">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="2">
         <v>13</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="2">
         <v>25</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="3">
         <v>607.28353995035195</v>
       </c>
@@ -1259,20 +1259,20 @@
         <v>212.75</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:16">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="2">
         <v>20</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="13">
         <v>325</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="3">
         <v>607.45009185766196</v>
       </c>
@@ -1303,18 +1303,18 @@
         <v>167.5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="17" spans="1:16">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="3">
         <v>17</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="2">
         <v>25</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="3">
         <v>607.28319410582401</v>
       </c>
@@ -1345,26 +1345,26 @@
         <v>160.25</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+    <row r="18" spans="1:16">
+      <c r="A18" s="13">
         <v>1</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="D18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="11">
+      <c r="E18" s="13">
+        <v>15</v>
+      </c>
+      <c r="F18" s="13">
         <v>650</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="13">
         <v>600</v>
       </c>
       <c r="H18" s="9">
@@ -1397,16 +1397,16 @@
         <v>214.75</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+    <row r="19" spans="1:16">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="2">
         <v>2</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="9">
         <v>607.62365758088299</v>
       </c>
@@ -1437,18 +1437,18 @@
         <v>213.25</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:16">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13">
         <v>740</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="3">
         <v>607.29199896525597</v>
       </c>
@@ -1479,16 +1479,16 @@
         <v>269.5</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+    <row r="21" spans="1:16">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="2">
         <v>6</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="3">
         <v>607.28948483679801</v>
       </c>
@@ -1519,16 +1519,16 @@
         <v>245.75</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+    <row r="22" spans="1:16">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="2">
         <v>8</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13">
         <v>300</v>
       </c>
       <c r="H22" s="3">
@@ -1561,16 +1561,16 @@
         <v>439.25</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+    <row r="23" spans="1:16">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="2">
         <v>9</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="3">
         <v>607.45680033490305</v>
       </c>
@@ -1601,18 +1601,18 @@
         <v>338</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+    <row r="24" spans="1:16">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="2">
         <v>11</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13">
         <v>650</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="13"/>
       <c r="H24" s="3">
         <v>607.289177218757</v>
       </c>
@@ -1643,16 +1643,16 @@
         <v>316.5</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:16">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="2">
         <v>12</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="3">
         <v>607.45454342637504</v>
       </c>
@@ -1683,24 +1683,24 @@
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11">
+    <row r="26" spans="1:16">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13">
         <v>2</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="11">
+      <c r="D26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13">
         <v>20</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="13">
         <v>400</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="13">
         <v>1200</v>
       </c>
       <c r="H26" s="9">
@@ -1733,16 +1733,16 @@
         <v>163.75</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+    <row r="27" spans="1:16">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2">
         <v>3</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
       <c r="H27" s="9">
         <v>607.29148017831403</v>
       </c>
@@ -1773,18 +1773,18 @@
         <v>246.25</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+    <row r="28" spans="1:16">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11">
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13">
         <v>300</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="13"/>
       <c r="H28" s="3">
         <v>607.622594834354</v>
       </c>
@@ -1815,16 +1815,16 @@
         <v>124.75</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+    <row r="29" spans="1:16">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="2">
         <v>6</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="3">
         <v>607.45312381139104</v>
       </c>
@@ -1855,20 +1855,20 @@
         <v>151.5</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+    <row r="30" spans="1:16">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="2">
         <v>11</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11">
+      <c r="D30" s="13"/>
+      <c r="E30" s="13">
         <v>15</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="13">
         <v>400</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="13">
         <v>600</v>
       </c>
       <c r="H30" s="3">
@@ -1901,16 +1901,16 @@
         <v>263.5</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+    <row r="31" spans="1:16">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="2">
         <v>12</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="3">
         <v>607.28871207739701</v>
       </c>
@@ -1941,18 +1941,18 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+    <row r="32" spans="1:16">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="3">
         <v>14</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11">
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
         <v>300</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="3">
         <v>607.28737022636801</v>
       </c>
@@ -1983,16 +1983,16 @@
         <v>177.25</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+    <row r="33" spans="1:16">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="3">
         <v>15</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="3">
         <v>607.28602605823505</v>
       </c>
@@ -2023,26 +2023,26 @@
         <v>184.25</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+    <row r="34" spans="1:16">
+      <c r="A34" s="13">
         <v>4</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="13">
         <v>1</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="11">
+      <c r="D34" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="11">
+      <c r="E34" s="13">
+        <v>15</v>
+      </c>
+      <c r="F34" s="13">
         <v>600</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="13">
         <v>600</v>
       </c>
       <c r="H34" s="3">
@@ -2075,16 +2075,16 @@
         <v>196.25</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+    <row r="35" spans="1:16">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="2">
         <v>2</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="3">
         <v>607.30245337632505</v>
       </c>
@@ -2115,18 +2115,18 @@
         <v>207.5</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+    <row r="36" spans="1:16">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="2">
         <v>3</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11">
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13">
         <v>750</v>
       </c>
-      <c r="G36" s="11"/>
+      <c r="G36" s="13"/>
       <c r="H36" s="3">
         <v>607.64704724529099</v>
       </c>
@@ -2157,16 +2157,16 @@
         <v>304.5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
+    <row r="37" spans="1:16">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="2">
         <v>4</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
       <c r="H37" s="3">
         <v>607.64494254176896</v>
       </c>
@@ -2197,16 +2197,16 @@
         <v>256.25</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
+    <row r="38" spans="1:16">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="2">
         <v>5</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13">
         <v>300</v>
       </c>
       <c r="H38" s="3">
@@ -2239,16 +2239,16 @@
         <v>518</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+    <row r="39" spans="1:16">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="2">
         <v>6</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
       <c r="H39" s="3">
         <v>607.14733366145197</v>
       </c>
@@ -2279,18 +2279,18 @@
         <v>320.25</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
+    <row r="40" spans="1:16">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="2">
         <v>7</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11">
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13">
         <v>600</v>
       </c>
-      <c r="G40" s="11"/>
+      <c r="G40" s="13"/>
       <c r="H40" s="3">
         <v>607.30401554938499</v>
       </c>
@@ -2321,16 +2321,16 @@
         <v>231.5</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
+    <row r="41" spans="1:16">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="2">
         <v>8</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
       <c r="H41" s="3">
         <v>607.46787730740903</v>
       </c>
@@ -2361,24 +2361,24 @@
         <v>200.5</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11">
+    <row r="42" spans="1:16">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13">
         <v>2</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="11">
+      <c r="D42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="13">
         <v>20</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="13">
         <v>400</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="13">
         <v>1200</v>
       </c>
       <c r="H42" s="3">
@@ -2411,16 +2411,16 @@
         <v>201.5</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
+    <row r="43" spans="1:16">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="2">
         <v>2</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="3">
         <v>607.135120639006</v>
       </c>
@@ -2451,18 +2451,18 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
+    <row r="44" spans="1:16">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="2">
         <v>3</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11">
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13">
         <v>300</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="13"/>
       <c r="H44" s="3">
         <v>607.29669987921602</v>
       </c>
@@ -2493,16 +2493,16 @@
         <v>140.5</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
+    <row r="45" spans="1:16">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
       <c r="H45" s="3">
         <v>607.12989883761702</v>
       </c>
@@ -2533,20 +2533,20 @@
         <v>145</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
+    <row r="46" spans="1:16">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2">
         <v>6</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11">
+      <c r="D46" s="13"/>
+      <c r="E46" s="13">
         <v>15</v>
       </c>
-      <c r="F46" s="11">
+      <c r="F46" s="13">
         <v>300</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="13">
         <v>600</v>
       </c>
       <c r="H46" s="3">
@@ -2579,16 +2579,16 @@
         <v>166.75</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
+    <row r="47" spans="1:16">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="2">
         <v>7</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
       <c r="H47" s="3">
         <v>607.46688158232405</v>
       </c>
@@ -2619,18 +2619,18 @@
         <v>171.25</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
+    <row r="48" spans="1:16">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="3">
         <v>8</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11">
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13">
         <v>400</v>
       </c>
-      <c r="G48" s="11"/>
+      <c r="G48" s="13"/>
       <c r="H48" s="3">
         <v>607.133179171135</v>
       </c>
@@ -2661,16 +2661,16 @@
         <v>259.75</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
+    <row r="49" spans="1:16">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="3">
         <v>9</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
       <c r="H49" s="3">
         <v>607.30209751854102</v>
       </c>
@@ -2720,6 +2720,10 @@
     <mergeCell ref="D26:D33"/>
     <mergeCell ref="E30:E33"/>
     <mergeCell ref="E26:E29"/>
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="D42:D49"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E46:E49"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="F30:F31"/>
@@ -2731,6 +2735,8 @@
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="B10:B17"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="G14:G17"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="D2:D9"/>
@@ -2738,26 +2744,20 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="D10:D17"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G17"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="D42:D49"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G45"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="G34:G37"/>
     <mergeCell ref="F36:F39"/>
     <mergeCell ref="G38:G41"/>
     <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="E46:E49"/>
     <mergeCell ref="F46:F47"/>
     <mergeCell ref="G46:G49"/>
     <mergeCell ref="F48:F49"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="F44:F45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2768,11 +2768,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57621B14-7309-4E78-AD67-5664E6F728F4}">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -2797,12 +2797,12 @@
     <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -2814,77 +2814,77 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="11">
+      <c r="F2" s="15">
+        <v>15</v>
+      </c>
+      <c r="G2" s="13">
         <v>650</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="13">
         <v>600</v>
       </c>
       <c r="I2" s="10"/>
@@ -2919,17 +2919,17 @@
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+    <row r="3" spans="1:21">
+      <c r="A3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10" t="e">
         <f t="shared" ref="J3:J5" si="0">10000000*(532-I3)/(532*I3)</f>
@@ -2962,25 +2962,25 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11">
+    <row r="4" spans="1:21">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13">
         <v>2</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="13">
+      <c r="E4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="15">
         <v>20</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="13">
         <v>400</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="13">
         <v>1200</v>
       </c>
       <c r="I4" s="10"/>
@@ -3015,17 +3015,17 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+    <row r="5" spans="1:21">
+      <c r="A5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10" t="e">
         <f t="shared" si="0"/>
@@ -3058,10 +3058,10 @@
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11" t="s">
-        <v>18</v>
+    <row r="6" spans="1:21">
+      <c r="A6" s="14"/>
+      <c r="B6" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -3070,7 +3070,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F6" s="7">
         <v>15</v>
@@ -3081,41 +3081,41 @@
       <c r="H6" s="7">
         <v>300</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="e">
+      <c r="I6" s="12"/>
+      <c r="J6" s="12" t="e">
         <f>10000000*(487.79-I6)/(487.79*I6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16" t="e">
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="e">
         <f>10000000*(487.79-K6)/(487.79*K6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="16" t="e">
+      <c r="M6" s="12" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16" t="e">
+      <c r="N6" s="12"/>
+      <c r="O6" s="12" t="e">
         <f>10000000*(487.79-N6)/(487.79*N6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16" t="e">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12" t="e">
         <f>10000000*(487.79-P6)/(487.79*P6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R6" s="16" t="e">
+      <c r="R6" s="12" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="2">
         <v>2</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2">
         <v>10</v>
@@ -3134,42 +3134,56 @@
       <c r="H7" s="2">
         <v>600</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="e">
+      <c r="I7" s="8">
+        <v>507.47998383489897</v>
+      </c>
+      <c r="J7" s="8">
         <f t="shared" ref="J7:J13" si="5">10000000*(487.79-I7)/(487.79*I7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="e">
+        <v>-795.41458384819168</v>
+      </c>
+      <c r="K7" s="8">
+        <v>507.897887847351</v>
+      </c>
+      <c r="L7" s="8">
         <f t="shared" ref="L7:L13" si="6">10000000*(487.79-K7)/(487.79*K7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="8" t="e">
+        <v>-811.62824964323829</v>
+      </c>
+      <c r="M7" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8" t="e">
+        <v>16.213665795046609</v>
+      </c>
+      <c r="N7" s="8">
+        <v>507.87014928898998</v>
+      </c>
+      <c r="O7" s="8">
         <f t="shared" ref="O7:Q9" si="7">10000000*(487.79-N7)/(487.79*N7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8" t="e">
+        <v>-810.55288738054583</v>
+      </c>
+      <c r="P7" s="8">
+        <v>507.91309202637598</v>
+      </c>
+      <c r="Q7" s="8">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="8" t="e">
+        <v>-812.21763203996159</v>
+      </c>
+      <c r="R7" s="8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>1.66474465941576</v>
+      </c>
+      <c r="S7" s="8">
+        <v>9</v>
+      </c>
+      <c r="T7" s="8">
+        <v>10.5</v>
+      </c>
+      <c r="U7" s="8">
+        <v>126.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="14"/>
+      <c r="B8" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -3178,7 +3192,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5">
         <v>10</v>
@@ -3189,41 +3203,55 @@
       <c r="H8" s="7">
         <v>600</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="e">
+      <c r="I8" s="8">
+        <v>507.43135737689403</v>
+      </c>
+      <c r="J8" s="8">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8" t="e">
+        <v>-793.52626026327005</v>
+      </c>
+      <c r="K8" s="8">
+        <v>507.42215802414199</v>
+      </c>
+      <c r="L8" s="8">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="8" t="e">
+        <v>-793.16897875193979</v>
+      </c>
+      <c r="M8" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8" t="e">
+        <v>-0.35728151133025676</v>
+      </c>
+      <c r="N8" s="8">
+        <v>507.42567619006701</v>
+      </c>
+      <c r="O8" s="8">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8" t="e">
+        <v>-793.30561768142775</v>
+      </c>
+      <c r="P8" s="8">
+        <v>507.41490300654698</v>
+      </c>
+      <c r="Q8" s="8">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="8" t="e">
+        <v>-792.88720156862883</v>
+      </c>
+      <c r="R8" s="8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
+        <v>-0.41841611279892277</v>
+      </c>
+      <c r="S8" s="8">
+        <v>1</v>
+      </c>
+      <c r="T8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="U8" s="8">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2">
         <v>2</v>
       </c>
@@ -3231,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6">
         <v>400</v>
@@ -3242,44 +3270,58 @@
       <c r="H9" s="7">
         <v>600</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="e">
+      <c r="I9" s="8">
+        <v>507.45443362678799</v>
+      </c>
+      <c r="J9" s="8">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8" t="e">
+        <v>-794.42243125179027</v>
+      </c>
+      <c r="K9" s="8">
+        <v>507.47037912461701</v>
+      </c>
+      <c r="L9" s="8">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="8" t="e">
+        <v>-795.04163037649721</v>
+      </c>
+      <c r="M9" s="8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8" t="e">
+        <v>0.61919912470693816</v>
+      </c>
+      <c r="N9" s="8">
+        <v>507.48266905408502</v>
+      </c>
+      <c r="O9" s="8">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8" t="e">
+        <v>-795.51884910299475</v>
+      </c>
+      <c r="P9" s="8">
+        <v>507.845007989066</v>
+      </c>
+      <c r="Q9" s="8">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="8" t="e">
+        <v>-809.57811356671425</v>
+      </c>
+      <c r="R9" s="8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>18</v>
+        <v>14.059264463719501</v>
+      </c>
+      <c r="S9" s="8">
+        <v>3.25</v>
+      </c>
+      <c r="T9" s="8">
+        <v>5.75</v>
+      </c>
+      <c r="U9" s="8">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
@@ -3288,7 +3330,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7">
         <v>15</v>
@@ -3299,41 +3341,41 @@
       <c r="H10" s="7">
         <v>300</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16" t="e">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12" t="e">
         <f>10000000*(487.79-I10)/(487.79*I10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16" t="e">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12" t="e">
         <f>10000000*(487.79-K10)/(487.79*K10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="16" t="e">
+      <c r="M10" s="12" t="e">
         <f t="shared" ref="M10:M13" si="8">J10-L10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16" t="e">
+      <c r="N10" s="12"/>
+      <c r="O10" s="12" t="e">
         <f>10000000*(487.79-N10)/(487.79*N10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16" t="e">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="e">
         <f>10000000*(487.79-P10)/(487.79*P10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R10" s="16" t="e">
+      <c r="R10" s="12" t="e">
         <f t="shared" ref="R10:R13" si="9">O10-Q10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="11"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2">
         <v>2</v>
       </c>
@@ -3341,7 +3383,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2">
         <v>10</v>
@@ -3384,10 +3426,10 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="11" t="s">
-        <v>19</v>
+    <row r="12" spans="1:21">
+      <c r="A12" s="14"/>
+      <c r="B12" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -3396,7 +3438,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F12" s="5">
         <v>10</v>
@@ -3439,9 +3481,9 @@
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="11"/>
+    <row r="13" spans="1:21">
+      <c r="A13" s="14"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="2">
         <v>2</v>
       </c>
@@ -3449,7 +3491,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F13" s="6">
         <v>400</v>

</xml_diff>